<commit_message>
updating writexls to output df for author and topic columns
</commit_message>
<xml_diff>
--- a/citations/test_df.xlsx
+++ b/citations/test_df.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AP2"/>
+  <dimension ref="A1:AQ2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -360,210 +360,215 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>UA_authored_year</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>display_name</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>author</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>ab</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>publication_date</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>so</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>so_id</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>host_organization</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>issn_l</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>url</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>pdf_url</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>license</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>version</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>first_page</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>last_page</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>volume</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>issue</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>is_oa</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>is_oa_anywhere</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>oa_status</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>oa_url</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>any_repository_has_fulltext</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>language</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>grants</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>cited_by_count</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>counts_by_year</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>publication_year</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>cited_by_api_url</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>ids</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>doi</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>type</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>referenced_works</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>related_works</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>is_paratext</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>is_retracted</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>concepts</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>topics</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>topic</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>subfield</t>
         </is>
       </c>
-      <c r="AO1" s="1" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>field</t>
         </is>
       </c>
-      <c r="AP1" s="1" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>domain</t>
         </is>
@@ -572,205 +577,210 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>https://openalex.org/W4210835162</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>The Glasgow Climate Conference (COP26)</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>The Glasgow Climate Conference (COP26)</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>https://openalex.org/A5087355631: Mitchell Lennan: https://orcid.org/0000-0003-4744-4496: first: FALSE: PhD Researcher, Strathclyde Law School, University of Strathclyde Glasgow United Kingdom: https://openalex.org/I181647926: University of Strathclyde: https://ror.org/00n3w3b69: GB: education: https://openalex.org/I181647926; https://openalex.org/A5071843257: Elisa Morgera: https://orcid.org/0000-0002-5234-8784: last: FALSE: Director, GCRF UKRI One Ocean Hub: https://openalex.org/I181647926: University of Strathclyde: https://ror.org/00n3w3b69: GB: education: https://openalex.org/I181647926</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>Abstract After over a decade of international efforts to include the ocean in the policy discussions at the United Nations Framework Convention on Climate Change ( UNFCCC ) annual Conference of the Parties ( COP ), the ocean has finally been included by, inter alia , a reference to ‘ocean-based action’ in a series of COP outcomes, notable among which is the cover decisions known as the ‘Glasgow Climate Pact’. This article provides the necessary background to the inclusion of the ocean in COP 26 outcomes, including the Pact, and examines key issues, impacts and shortfalls of the Pact and other COP 26 outcomes, including mitigation, adaptation, finance and human rights. It concludes with suggestions for priority research areas moving forward.</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>2022-02-07</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>The International Journal of Marine and Coastal Law</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>https://openalex.org/S20683218</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>Brill</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>0927-3522</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="L2" t="inlineStr">
         <is>
           <t>https://doi.org/10.1163/15718085-bja10083</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="M2" t="inlineStr">
         <is>
           <t>https://brill.com/downloadpdf/journals/estu/37/1/article-p137_6.pdf</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="N2" t="inlineStr">
         <is>
           <t>cc-by</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
+      <c r="O2" t="inlineStr">
         <is>
           <t>publishedVersion</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr">
+      <c r="P2" t="inlineStr">
         <is>
           <t>137</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
+      <c r="Q2" t="inlineStr">
         <is>
           <t>151</t>
         </is>
       </c>
-      <c r="Q2" t="inlineStr">
+      <c r="R2" t="inlineStr">
         <is>
           <t>37</t>
         </is>
       </c>
-      <c r="R2" t="inlineStr">
+      <c r="S2" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="S2" t="inlineStr">
+      <c r="T2" t="inlineStr">
         <is>
           <t>TRUE</t>
         </is>
       </c>
-      <c r="T2" t="inlineStr">
+      <c r="U2" t="inlineStr">
         <is>
           <t>TRUE</t>
         </is>
       </c>
-      <c r="U2" t="inlineStr">
+      <c r="V2" t="inlineStr">
         <is>
           <t>hybrid</t>
         </is>
       </c>
-      <c r="V2" t="inlineStr">
+      <c r="W2" t="inlineStr">
         <is>
           <t>https://brill.com/downloadpdf/journals/estu/37/1/article-p137_6.pdf</t>
         </is>
       </c>
-      <c r="W2" t="inlineStr">
+      <c r="X2" t="inlineStr">
         <is>
           <t>TRUE</t>
         </is>
       </c>
-      <c r="X2" t="inlineStr">
+      <c r="Y2" t="inlineStr">
         <is>
           <t>en</t>
         </is>
       </c>
-      <c r="Z2" t="inlineStr">
+      <c r="AA2" t="inlineStr">
         <is>
           <t>58</t>
         </is>
       </c>
-      <c r="AA2" t="inlineStr">
+      <c r="AB2" t="inlineStr">
         <is>
           <t>2024: 2023: 2022: 30: 19: 9</t>
         </is>
       </c>
-      <c r="AB2" t="inlineStr">
+      <c r="AC2" t="inlineStr">
         <is>
           <t>2022</t>
         </is>
       </c>
-      <c r="AC2" t="inlineStr">
+      <c r="AD2" t="inlineStr">
         <is>
           <t>https://api.openalex.org/works?filter=cites:W4210835162</t>
         </is>
       </c>
-      <c r="AD2" t="inlineStr">
+      <c r="AE2" t="inlineStr">
         <is>
           <t>https://openalex.org/W4210835162: https://doi.org/10.1163/15718085-bja10083</t>
         </is>
       </c>
-      <c r="AE2" t="inlineStr">
+      <c r="AF2" t="inlineStr">
         <is>
           <t>https://doi.org/10.1163/15718085-bja10083</t>
         </is>
       </c>
-      <c r="AF2" t="inlineStr">
+      <c r="AG2" t="inlineStr">
         <is>
           <t>article</t>
         </is>
       </c>
-      <c r="AG2" t="inlineStr">
+      <c r="AH2" t="inlineStr">
         <is>
           <t>https://openalex.org/W2980737502</t>
         </is>
       </c>
-      <c r="AH2" t="inlineStr">
+      <c r="AI2" t="inlineStr">
         <is>
           <t>https://openalex.org/W4233921916: https://openalex.org/W3148144928: https://openalex.org/W2575112651: https://openalex.org/W235433852: https://openalex.org/W2119377653: https://openalex.org/W2068081422: https://openalex.org/W2020757966: https://openalex.org/W2005847371: https://openalex.org/W187456812: https://openalex.org/W1615167197</t>
         </is>
       </c>
-      <c r="AI2" t="inlineStr">
+      <c r="AJ2" t="inlineStr">
         <is>
           <t>FALSE</t>
         </is>
       </c>
-      <c r="AJ2" t="inlineStr">
+      <c r="AK2" t="inlineStr">
         <is>
           <t>FALSE</t>
         </is>
       </c>
-      <c r="AK2" t="inlineStr">
+      <c r="AL2" t="inlineStr">
         <is>
           <t>https://openalex.org/C2779073994: https://openalex.org/C17744445: https://openalex.org/C2780608745: https://openalex.org/C132651083: https://openalex.org/C2778539042: https://openalex.org/C199539241: https://openalex.org/C99743013: https://openalex.org/C111368507: https://openalex.org/C127313418: https://www.wikidata.org/wiki/Q1751686: https://www.wikidata.org/wiki/Q36442: https://www.wikidata.org/wiki/Q367293: https://www.wikidata.org/wiki/Q7942: https://www.wikidata.org/wiki/Q208645: https://www.wikidata.org/wiki/Q7748: https://www.wikidata.org/wiki/Q47359: https://www.wikidata.org/wiki/Q43518: https://www.wikidata.org/wiki/Q1069: Pact: Political science: Convention: Climate change: United Nations Framework Convention on Climate Change: Law: Kyoto Protocol: Oceanography: Geology: 2: 0: 2: 2: 4: 1: 3: 1: 0: 0.68293977: 0.58795327: 0.5614837: 0.50553393: 0.50141287: 0.18397388: 0.11712614: 0.11092797: 0</t>
         </is>
       </c>
-      <c r="AL2" t="inlineStr">
+      <c r="AM2" t="inlineStr">
         <is>
           <t>1: 0.9507: topic: https://openalex.org/T12414: Coastal and Marine Management; 1: 0.9507: subfield: https://openalex.org/subfields/2308: Management, Monitoring, Policy and Law; 1: 0.9507: field: https://openalex.org/fields/23: Environmental Science; 1: 0.9507: domain: https://openalex.org/domains/3: Physical Sciences</t>
         </is>
       </c>
-      <c r="AM2" t="inlineStr">
+      <c r="AN2" t="inlineStr">
         <is>
           <t>Coastal and Marine Management</t>
         </is>
       </c>
-      <c r="AN2" t="inlineStr">
+      <c r="AO2" t="inlineStr">
         <is>
           <t>Management, Monitoring, Policy and Law</t>
         </is>
       </c>
-      <c r="AO2" t="inlineStr">
+      <c r="AP2" t="inlineStr">
         <is>
           <t>Environmental Science</t>
         </is>
       </c>
-      <c r="AP2" t="inlineStr">
+      <c r="AQ2" t="inlineStr">
         <is>
           <t>Physical Sciences</t>
         </is>

</xml_diff>